<commit_message>
Added other character's sheet
</commit_message>
<xml_diff>
--- a/Ficha de STARS - 4.0.xlsx
+++ b/Ficha de STARS - 4.0.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr codeName="EstaPastaDeTrabalho"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgmde\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\RPG\STARS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28E8358-9A6C-4B98-98AD-7660C5C1D2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87A7720-D4B1-4B0F-A6BE-965D82C1DE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5948357-C3D8-430D-9A83-EF9F6AD52DE5}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{F5948357-C3D8-430D-9A83-EF9F6AD52DE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Básico" sheetId="1" r:id="rId1"/>
     <sheet name="Equipamento" sheetId="4" r:id="rId2"/>
-    <sheet name="Outros" sheetId="7" r:id="rId3"/>
+    <sheet name="Outros" sheetId="7" state="hidden" r:id="rId3"/>
     <sheet name="Rank" sheetId="6" state="hidden" r:id="rId4"/>
     <sheet name="Tipos das Armas" sheetId="5" state="hidden" r:id="rId5"/>
     <sheet name="Treinamento" sheetId="3" state="hidden" r:id="rId6"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="182">
   <si>
     <t>Características Básicas</t>
   </si>
@@ -587,31 +587,7 @@
     <t>X%</t>
   </si>
   <si>
-    <t>Dado</t>
-  </si>
-  <si>
-    <t>Quantidade (Inteiro)</t>
-  </si>
-  <si>
-    <t>Rolagem de Dados</t>
-  </si>
-  <si>
-    <t>Perícia (+ Mod)</t>
-  </si>
-  <si>
-    <t>Tipo (Maior, menor...)</t>
-  </si>
-  <si>
-    <t>d6</t>
-  </si>
-  <si>
-    <t>Soma</t>
-  </si>
-  <si>
-    <t>Maior</t>
-  </si>
-  <si>
-    <t>Menor</t>
+    <t>Espaço Extra</t>
   </si>
 </sst>
 </file>
@@ -621,7 +597,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -780,19 +756,6 @@
       <name val="Algerian"/>
       <family val="5"/>
     </font>
-    <font>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Agency FB"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -850,7 +813,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="64">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -1578,26 +1541,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thick">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1788,6 +1736,177 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1797,6 +1916,99 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="23" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1805,297 +2017,6 @@
     </xf>
     <xf numFmtId="164" fontId="23" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="21" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="21" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="21" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3192,41 +3113,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B3E8BF-9144-4CFE-B336-607C81302F71}">
-  <sheetPr codeName="Planilha1"/>
   <dimension ref="B1:V58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34:L40"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.109375" customWidth="1"/>
-    <col min="12" max="15" width="15.6640625" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" customWidth="1"/>
-    <col min="18" max="18" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.140625" customWidth="1"/>
+    <col min="12" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:22" ht="22.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="97"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="99"/>
-      <c r="F2" s="106" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="107"/>
-      <c r="H2" s="108"/>
-      <c r="J2" s="76" t="s">
+    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:22" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="117"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="119"/>
+      <c r="F2" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="127"/>
+      <c r="H2" s="128"/>
+      <c r="J2" s="133" t="s">
         <v>49</v>
       </c>
       <c r="L2" s="14" t="s">
@@ -3260,14 +3180,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="100"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="102"/>
+    <row r="3" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="120"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="122"/>
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="J3" s="77"/>
+      <c r="J3" s="134"/>
       <c r="L3" s="29" t="s">
         <v>16</v>
       </c>
@@ -3299,17 +3219,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="100"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="102"/>
+    <row r="4" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="120"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="122"/>
       <c r="E4" s="11"/>
       <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="89"/>
-      <c r="J4" s="77"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="101"/>
+      <c r="J4" s="134"/>
       <c r="L4" s="29" t="s">
         <v>17</v>
       </c>
@@ -3341,14 +3261,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="100"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="102"/>
+    <row r="5" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="120"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="122"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="J5" s="77"/>
+      <c r="J5" s="134"/>
       <c r="L5" s="29" t="s">
         <v>18</v>
       </c>
@@ -3380,16 +3300,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="100"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="102"/>
+    <row r="6" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="120"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="122"/>
       <c r="F6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="89"/>
-      <c r="J6" s="77"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="101"/>
+      <c r="J6" s="134"/>
       <c r="L6" s="29" t="s">
         <v>19</v>
       </c>
@@ -3421,14 +3341,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="100"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="102"/>
+    <row r="7" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="120"/>
+      <c r="C7" s="121"/>
+      <c r="D7" s="122"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="J7" s="77"/>
+      <c r="J7" s="134"/>
       <c r="L7" s="29" t="s">
         <v>20</v>
       </c>
@@ -3460,19 +3380,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="100"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="102"/>
+    <row r="8" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="120"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="122"/>
       <c r="F8" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="109" t="str">
+      <c r="G8" s="129" t="str">
         <f>IF(AND(G6&gt;=8,G6&lt;=12),"Criança",IF(AND(G6&gt;=13,G6&lt;=17),"Adolescente",IF(AND(G6&gt;=18,G6&lt;=24),"Jovem Adulto",IF(AND(G6&gt;=25,G6&lt;=39),"Adulto",IF(AND(G6&gt;=40,G6&lt;=64),"Velho",IF(G6&gt;=65,"Idoso","Bebê de Potinho"))))))</f>
         <v>Bebê de Potinho</v>
       </c>
-      <c r="H8" s="110"/>
-      <c r="J8" s="77"/>
+      <c r="H8" s="130"/>
+      <c r="J8" s="134"/>
       <c r="L8" s="29" t="s">
         <v>21</v>
       </c>
@@ -3504,14 +3424,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="100"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="102"/>
+    <row r="9" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="120"/>
+      <c r="C9" s="121"/>
+      <c r="D9" s="122"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="J9" s="77"/>
+      <c r="J9" s="134"/>
       <c r="L9" s="30" t="s">
         <v>22</v>
       </c>
@@ -3543,16 +3463,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:22" ht="15" x14ac:dyDescent="0.3">
-      <c r="B10" s="100"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="102"/>
+    <row r="10" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="120"/>
+      <c r="C10" s="121"/>
+      <c r="D10" s="122"/>
       <c r="F10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="111"/>
-      <c r="H10" s="112"/>
-      <c r="J10" s="77"/>
+      <c r="G10" s="131"/>
+      <c r="H10" s="132"/>
+      <c r="J10" s="134"/>
       <c r="R10" s="26" t="s">
         <v>64</v>
       </c>
@@ -3568,14 +3488,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:22" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B11" s="100"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="102"/>
+    <row r="11" spans="2:22" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="120"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="122"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="J11" s="77"/>
+      <c r="J11" s="134"/>
       <c r="L11" s="22" t="s">
         <v>13</v>
       </c>
@@ -3606,16 +3526,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="100"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="102"/>
+    <row r="12" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="120"/>
+      <c r="C12" s="121"/>
+      <c r="D12" s="122"/>
       <c r="F12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="96"/>
-      <c r="H12" s="89"/>
-      <c r="J12" s="77"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="101"/>
+      <c r="J12" s="134"/>
       <c r="L12" s="17" t="s">
         <v>40</v>
       </c>
@@ -3644,14 +3564,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="100"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="102"/>
+    <row r="13" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="120"/>
+      <c r="C13" s="121"/>
+      <c r="D13" s="122"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="J13" s="77"/>
+      <c r="J13" s="134"/>
       <c r="L13" s="29" t="s">
         <v>39</v>
       </c>
@@ -3680,16 +3600,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="100"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="102"/>
+    <row r="14" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="120"/>
+      <c r="C14" s="121"/>
+      <c r="D14" s="122"/>
       <c r="F14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="96"/>
-      <c r="H14" s="89"/>
-      <c r="J14" s="77"/>
+      <c r="G14" s="100"/>
+      <c r="H14" s="101"/>
+      <c r="J14" s="134"/>
       <c r="L14" s="20" t="s">
         <v>38</v>
       </c>
@@ -3718,14 +3638,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B15" s="100"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="102"/>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="120"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="122"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="J15" s="77"/>
+      <c r="J15" s="134"/>
       <c r="R15" s="26" t="s">
         <v>68</v>
       </c>
@@ -3741,16 +3661,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:22" ht="15" x14ac:dyDescent="0.3">
-      <c r="B16" s="100"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="102"/>
+    <row r="16" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="120"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="122"/>
       <c r="F16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="94"/>
-      <c r="H16" s="95"/>
-      <c r="J16" s="77"/>
+      <c r="G16" s="115"/>
+      <c r="H16" s="116"/>
+      <c r="J16" s="134"/>
       <c r="L16" s="33" t="s">
         <v>43</v>
       </c>
@@ -3781,25 +3701,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="100"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="102"/>
+    <row r="17" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="120"/>
+      <c r="C17" s="121"/>
+      <c r="D17" s="122"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="J17" s="77"/>
-      <c r="L17" s="85">
+      <c r="J17" s="134"/>
+      <c r="L17" s="136">
         <f>5 + P5+ M17</f>
         <v>5</v>
       </c>
-      <c r="M17" s="82"/>
-      <c r="N17" s="85">
+      <c r="M17" s="139"/>
+      <c r="N17" s="136">
         <f>5+(G22/5%)/2+O17+P6</f>
         <v>5</v>
       </c>
-      <c r="O17" s="82"/>
-      <c r="P17" s="79" t="str">
+      <c r="O17" s="139"/>
+      <c r="P17" s="167" t="str">
         <f>IF(P16="Deslocamento (m)", _xlfn.VALUETOTEXT(9+IF(AND(G18="Duelista",G20="Tropa de Elite",G22&gt;=15%),3,0)+(ROUND(P5/2,0)*1.5)), _xlfn.VALUETOTEXT(((9+IF(AND(G18="Duelista",G20="Tropa de Elite",G22&gt;=15%),3,0)+(ROUND(P5/2,0)*1.5))/1.5)))</f>
         <v>9</v>
       </c>
@@ -3818,22 +3738,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="100"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="102"/>
+    <row r="18" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="120"/>
+      <c r="C18" s="121"/>
+      <c r="D18" s="122"/>
       <c r="E18" s="11"/>
       <c r="F18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="96"/>
-      <c r="H18" s="89"/>
-      <c r="J18" s="77"/>
-      <c r="L18" s="86"/>
-      <c r="M18" s="83"/>
-      <c r="N18" s="86"/>
-      <c r="O18" s="83"/>
-      <c r="P18" s="80"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="101"/>
+      <c r="J18" s="134"/>
+      <c r="L18" s="137"/>
+      <c r="M18" s="140"/>
+      <c r="N18" s="137"/>
+      <c r="O18" s="140"/>
+      <c r="P18" s="168"/>
       <c r="R18" s="26" t="s">
         <v>86</v>
       </c>
@@ -3849,19 +3769,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="100"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="102"/>
+    <row r="19" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="120"/>
+      <c r="C19" s="121"/>
+      <c r="D19" s="122"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-      <c r="J19" s="77"/>
-      <c r="L19" s="86"/>
-      <c r="M19" s="83"/>
-      <c r="N19" s="86"/>
-      <c r="O19" s="83"/>
-      <c r="P19" s="80"/>
+      <c r="J19" s="134"/>
+      <c r="L19" s="137"/>
+      <c r="M19" s="140"/>
+      <c r="N19" s="137"/>
+      <c r="O19" s="140"/>
+      <c r="P19" s="168"/>
       <c r="R19" s="26" t="s">
         <v>72</v>
       </c>
@@ -3877,22 +3797,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="100"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="102"/>
+    <row r="20" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="120"/>
+      <c r="C20" s="121"/>
+      <c r="D20" s="122"/>
       <c r="E20" s="11"/>
       <c r="F20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="96"/>
-      <c r="H20" s="89"/>
-      <c r="J20" s="77"/>
-      <c r="L20" s="87"/>
-      <c r="M20" s="84"/>
-      <c r="N20" s="87"/>
-      <c r="O20" s="84"/>
-      <c r="P20" s="81"/>
+      <c r="G20" s="100"/>
+      <c r="H20" s="101"/>
+      <c r="J20" s="134"/>
+      <c r="L20" s="138"/>
+      <c r="M20" s="141"/>
+      <c r="N20" s="138"/>
+      <c r="O20" s="141"/>
+      <c r="P20" s="169"/>
       <c r="R20" s="26" t="s">
         <v>73</v>
       </c>
@@ -3908,14 +3828,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B21" s="100"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="102"/>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="120"/>
+      <c r="C21" s="121"/>
+      <c r="D21" s="122"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
-      <c r="J21" s="77"/>
+      <c r="J21" s="134"/>
       <c r="R21" s="26" t="s">
         <v>74</v>
       </c>
@@ -3931,25 +3851,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:22" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="103"/>
-      <c r="C22" s="104"/>
-      <c r="D22" s="105"/>
+    <row r="22" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="123"/>
+      <c r="C22" s="124"/>
+      <c r="D22" s="125"/>
       <c r="E22" s="11"/>
       <c r="F22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="93"/>
-      <c r="H22" s="89"/>
-      <c r="J22" s="78"/>
-      <c r="L22" s="133" t="str">
-        <f>_xlfn.CONCAT("Limite de PP: ",(G22/5%) + IF(G20="Caminho da Agonia", P6, 0))</f>
+      <c r="G22" s="114"/>
+      <c r="H22" s="101"/>
+      <c r="J22" s="135"/>
+      <c r="L22" s="104" t="str">
+        <f>_xlfn.CONCAT("Limite de PP: ",(G22/5%)+P6)</f>
         <v>Limite de PP: 0</v>
       </c>
-      <c r="M22" s="133"/>
-      <c r="N22" s="133"/>
-      <c r="O22" s="133"/>
-      <c r="P22" s="133"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="104"/>
+      <c r="O22" s="104"/>
+      <c r="P22" s="104"/>
       <c r="R22" s="26" t="s">
         <v>75</v>
       </c>
@@ -3965,7 +3885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F23" s="4"/>
       <c r="R23" s="26" t="s">
         <v>76</v>
@@ -3982,21 +3902,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="90" t="s">
+    <row r="24" spans="2:22" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="111" t="s">
         <v>146</v>
       </c>
-      <c r="C24" s="91"/>
-      <c r="D24" s="92"/>
-      <c r="F24" s="90" t="s">
+      <c r="C24" s="112"/>
+      <c r="D24" s="113"/>
+      <c r="F24" s="111" t="s">
         <v>175</v>
       </c>
-      <c r="G24" s="91"/>
-      <c r="H24" s="92"/>
-      <c r="J24" s="119" t="s">
+      <c r="G24" s="112"/>
+      <c r="H24" s="113"/>
+      <c r="J24" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="L24" s="136" t="s">
+      <c r="L24" s="107" t="s">
         <v>50</v>
       </c>
       <c r="M24" s="14" t="s">
@@ -4005,10 +3925,10 @@
       <c r="N24" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="O24" s="138" t="s">
+      <c r="O24" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="P24" s="138"/>
+      <c r="P24" s="109"/>
       <c r="R24" s="26" t="s">
         <v>77</v>
       </c>
@@ -4024,7 +3944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
@@ -4034,15 +3954,15 @@
       <c r="D25" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="122"/>
-      <c r="G25" s="123"/>
-      <c r="H25" s="124"/>
-      <c r="J25" s="120"/>
-      <c r="L25" s="137"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="93"/>
+      <c r="J25" s="77"/>
+      <c r="L25" s="108"/>
       <c r="M25" s="66"/>
       <c r="N25" s="35"/>
-      <c r="O25" s="131"/>
-      <c r="P25" s="132"/>
+      <c r="O25" s="102"/>
+      <c r="P25" s="103"/>
       <c r="Q25" s="34"/>
       <c r="R25" s="26" t="s">
         <v>78</v>
@@ -4059,24 +3979,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="58"/>
       <c r="C26" s="59">
         <v>0.1</v>
       </c>
       <c r="D26" s="71"/>
-      <c r="F26" s="125"/>
-      <c r="G26" s="126"/>
-      <c r="H26" s="127"/>
-      <c r="J26" s="120"/>
-      <c r="L26" s="134">
+      <c r="F26" s="94"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="96"/>
+      <c r="J26" s="77"/>
+      <c r="L26" s="105">
         <f>((M9+N9)*3)+SUM(N25:N31)</f>
         <v>0</v>
       </c>
       <c r="M26" s="67"/>
       <c r="N26" s="34"/>
-      <c r="O26" s="131"/>
-      <c r="P26" s="132"/>
+      <c r="O26" s="102"/>
+      <c r="P26" s="103"/>
       <c r="Q26" s="34"/>
       <c r="R26" s="26" t="s">
         <v>79</v>
@@ -4093,21 +4013,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="C27" s="61">
         <v>0.2</v>
       </c>
       <c r="D27" s="70"/>
-      <c r="F27" s="125"/>
-      <c r="G27" s="126"/>
-      <c r="H27" s="127"/>
-      <c r="J27" s="120"/>
-      <c r="L27" s="135"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="96"/>
+      <c r="J27" s="77"/>
+      <c r="L27" s="106"/>
       <c r="M27" s="68"/>
       <c r="N27" s="28"/>
-      <c r="O27" s="131"/>
-      <c r="P27" s="132"/>
+      <c r="O27" s="102"/>
+      <c r="P27" s="103"/>
       <c r="Q27" s="34"/>
       <c r="R27" s="26" t="s">
         <v>80</v>
@@ -4124,21 +4044,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
       <c r="C28" s="61">
         <v>0.3</v>
       </c>
       <c r="D28" s="70"/>
-      <c r="F28" s="125"/>
-      <c r="G28" s="126"/>
-      <c r="H28" s="127"/>
-      <c r="J28" s="120"/>
-      <c r="L28" s="135"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="96"/>
+      <c r="J28" s="77"/>
+      <c r="L28" s="106"/>
       <c r="M28" s="69"/>
       <c r="N28" s="27"/>
-      <c r="O28" s="131"/>
-      <c r="P28" s="132"/>
+      <c r="O28" s="102"/>
+      <c r="P28" s="103"/>
       <c r="R28" s="26" t="s">
         <v>81</v>
       </c>
@@ -4154,21 +4074,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
       <c r="C29" s="61">
         <v>0.4</v>
       </c>
       <c r="D29" s="11"/>
-      <c r="F29" s="125"/>
-      <c r="G29" s="126"/>
-      <c r="H29" s="127"/>
-      <c r="J29" s="120"/>
-      <c r="L29" s="135"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="96"/>
+      <c r="J29" s="77"/>
+      <c r="L29" s="106"/>
       <c r="M29" s="69"/>
       <c r="N29" s="27"/>
-      <c r="O29" s="131"/>
-      <c r="P29" s="132"/>
+      <c r="O29" s="102"/>
+      <c r="P29" s="103"/>
       <c r="R29" s="26" t="s">
         <v>82</v>
       </c>
@@ -4184,21 +4104,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
       <c r="C30" s="61">
         <v>0.5</v>
       </c>
       <c r="D30" s="11"/>
-      <c r="F30" s="125"/>
-      <c r="G30" s="126"/>
-      <c r="H30" s="127"/>
-      <c r="J30" s="120"/>
-      <c r="L30" s="135"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="96"/>
+      <c r="J30" s="77"/>
+      <c r="L30" s="106"/>
       <c r="M30" s="68"/>
       <c r="N30" s="28"/>
-      <c r="O30" s="131"/>
-      <c r="P30" s="132"/>
+      <c r="O30" s="102"/>
+      <c r="P30" s="103"/>
       <c r="R30" s="26" t="s">
         <v>83</v>
       </c>
@@ -4208,38 +4128,36 @@
       <c r="T30" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="U30" s="38">
-        <v>7</v>
-      </c>
+      <c r="U30" s="38"/>
       <c r="V30" s="26">
         <f>VLOOKUP(S30,$L$3:$P$9,5,FALSE)+IF(Atributos[[#This Row],[Treinamento]] = "Leigo",0,IF(Atributos[[#This Row],[Treinamento]]="Calejado",2,IF(Atributos[[#This Row],[Treinamento]]="Experiente",3,4)))+Atributos[[#This Row],[Outros]]</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="10"/>
       <c r="C31" s="61">
         <v>0.6</v>
       </c>
       <c r="D31" s="11"/>
-      <c r="F31" s="128"/>
-      <c r="G31" s="129"/>
-      <c r="H31" s="130"/>
-      <c r="J31" s="121"/>
-      <c r="L31" s="135"/>
+      <c r="F31" s="97"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="99"/>
+      <c r="J31" s="78"/>
+      <c r="L31" s="106"/>
       <c r="M31" s="66"/>
       <c r="N31" s="35"/>
-      <c r="O31" s="131"/>
-      <c r="P31" s="132"/>
-    </row>
-    <row r="32" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O31" s="102"/>
+      <c r="P31" s="103"/>
+    </row>
+    <row r="32" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="10"/>
       <c r="C32" s="61">
         <v>0.7</v>
       </c>
       <c r="D32" s="11"/>
     </row>
-    <row r="33" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="10"/>
       <c r="C33" s="61">
         <v>0.8</v>
@@ -4254,7 +4172,7 @@
       <c r="H33" s="74" t="s">
         <v>158</v>
       </c>
-      <c r="J33" s="119" t="s">
+      <c r="J33" s="76" t="s">
         <v>166</v>
       </c>
       <c r="L33" s="33" t="s">
@@ -4273,7 +4191,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
       <c r="C34" s="61">
         <v>0.9</v>
@@ -4288,22 +4206,22 @@
       <c r="H34" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J34" s="120"/>
-      <c r="L34" s="139"/>
-      <c r="M34" s="142" t="s">
+      <c r="J34" s="77"/>
+      <c r="L34" s="79"/>
+      <c r="M34" s="82" t="s">
         <v>161</v>
       </c>
-      <c r="N34" s="139">
+      <c r="N34" s="79">
         <f>SUMIF(Resistencia_Elemental[Aplicável?],"SIM",Resistencia_Elemental[RD (n°)])+SUMIF(Resistencia_Fisico[Aplicável?],"SIM",Resistencia_Fisico[RD (n°)])</f>
         <v>0</v>
       </c>
-      <c r="O34" s="113">
+      <c r="O34" s="85">
         <f>($L$34-$N$34)/IF($M$34="SIM",2,1)</f>
         <v>0</v>
       </c>
-      <c r="P34" s="116"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P34" s="88"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="12"/>
       <c r="C35" s="64">
         <v>1</v>
@@ -4318,14 +4236,14 @@
       <c r="H35" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J35" s="120"/>
-      <c r="L35" s="140"/>
-      <c r="M35" s="143"/>
-      <c r="N35" s="140"/>
-      <c r="O35" s="114"/>
-      <c r="P35" s="117"/>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="J35" s="77"/>
+      <c r="L35" s="80"/>
+      <c r="M35" s="83"/>
+      <c r="N35" s="80"/>
+      <c r="O35" s="86"/>
+      <c r="P35" s="89"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F36" s="75" t="s">
         <v>157</v>
       </c>
@@ -4335,19 +4253,19 @@
       <c r="H36" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J36" s="120"/>
-      <c r="L36" s="140"/>
-      <c r="M36" s="143"/>
-      <c r="N36" s="140"/>
-      <c r="O36" s="114"/>
-      <c r="P36" s="117"/>
-    </row>
-    <row r="37" spans="2:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B37" s="90" t="s">
+      <c r="J36" s="77"/>
+      <c r="L36" s="80"/>
+      <c r="M36" s="83"/>
+      <c r="N36" s="80"/>
+      <c r="O36" s="86"/>
+      <c r="P36" s="89"/>
+    </row>
+    <row r="37" spans="2:16" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B37" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="91"/>
-      <c r="D37" s="92"/>
+      <c r="C37" s="112"/>
+      <c r="D37" s="113"/>
       <c r="F37" s="75" t="s">
         <v>19</v>
       </c>
@@ -4357,14 +4275,14 @@
       <c r="H37" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J37" s="120"/>
-      <c r="L37" s="140"/>
-      <c r="M37" s="143"/>
-      <c r="N37" s="140"/>
-      <c r="O37" s="114"/>
-      <c r="P37" s="117"/>
-    </row>
-    <row r="38" spans="2:16" ht="15" x14ac:dyDescent="0.3">
+      <c r="J37" s="77"/>
+      <c r="L37" s="80"/>
+      <c r="M37" s="83"/>
+      <c r="N37" s="80"/>
+      <c r="O37" s="86"/>
+      <c r="P37" s="89"/>
+    </row>
+    <row r="38" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
         <v>10</v>
       </c>
@@ -4383,14 +4301,14 @@
       <c r="H38" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J38" s="120"/>
-      <c r="L38" s="140"/>
-      <c r="M38" s="143"/>
-      <c r="N38" s="140"/>
-      <c r="O38" s="114"/>
-      <c r="P38" s="117"/>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="J38" s="77"/>
+      <c r="L38" s="80"/>
+      <c r="M38" s="83"/>
+      <c r="N38" s="80"/>
+      <c r="O38" s="86"/>
+      <c r="P38" s="89"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="58"/>
       <c r="C39" s="59">
         <v>0.05</v>
@@ -4407,14 +4325,14 @@
       <c r="H39" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J39" s="120"/>
-      <c r="L39" s="140"/>
-      <c r="M39" s="143"/>
-      <c r="N39" s="140"/>
-      <c r="O39" s="114"/>
-      <c r="P39" s="117"/>
-    </row>
-    <row r="40" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J39" s="77"/>
+      <c r="L39" s="80"/>
+      <c r="M39" s="83"/>
+      <c r="N39" s="80"/>
+      <c r="O39" s="86"/>
+      <c r="P39" s="89"/>
+    </row>
+    <row r="40" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="10"/>
       <c r="C40" s="61">
         <v>0.15</v>
@@ -4431,14 +4349,14 @@
       <c r="H40" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J40" s="121"/>
-      <c r="L40" s="141"/>
-      <c r="M40" s="144"/>
-      <c r="N40" s="141"/>
-      <c r="O40" s="115"/>
-      <c r="P40" s="118"/>
-    </row>
-    <row r="41" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J40" s="78"/>
+      <c r="L40" s="81"/>
+      <c r="M40" s="84"/>
+      <c r="N40" s="81"/>
+      <c r="O40" s="87"/>
+      <c r="P40" s="90"/>
+    </row>
+    <row r="41" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="10"/>
       <c r="C41" s="61">
         <v>0.25</v>
@@ -4447,7 +4365,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
       <c r="C42" s="61">
         <v>0.35</v>
@@ -4464,18 +4382,11 @@
       <c r="H42" s="74" t="s">
         <v>158</v>
       </c>
-      <c r="J42" s="119" t="s">
-        <v>183</v>
-      </c>
-      <c r="L42" s="170" t="s">
+      <c r="J42" s="76" t="s">
         <v>181</v>
       </c>
-      <c r="N42" s="172" t="s">
-        <v>181</v>
-      </c>
-      <c r="O42" s="173"/>
-    </row>
-    <row r="43" spans="2:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B43" s="10"/>
       <c r="C43" s="61">
         <v>0.45</v>
@@ -4492,18 +4403,9 @@
       <c r="H43" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J43" s="120"/>
-      <c r="L43" s="178" t="s">
-        <v>186</v>
-      </c>
-      <c r="M43" s="171"/>
-      <c r="N43" s="174">
-        <f ca="1">RANDBETWEEN(1,RIGHT(L43,LEN(L43)-1)) + IFERROR(VLOOKUP(L49,Atributos[],5,TRUE),0)</f>
-        <v>3</v>
-      </c>
-      <c r="O43" s="175"/>
-    </row>
-    <row r="44" spans="2:16" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J43" s="77"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="10"/>
       <c r="C44" s="61">
         <v>0.55000000000000004</v>
@@ -4520,15 +4422,9 @@
       <c r="H44" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J44" s="120"/>
-      <c r="L44" s="170" t="s">
-        <v>182</v>
-      </c>
-      <c r="M44" s="171"/>
-      <c r="N44" s="174"/>
-      <c r="O44" s="175"/>
-    </row>
-    <row r="45" spans="2:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="J44" s="77"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45" s="10"/>
       <c r="C45" s="61">
         <v>0.65</v>
@@ -4545,15 +4441,9 @@
       <c r="H45" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J45" s="120"/>
-      <c r="L45" s="178">
-        <v>2</v>
-      </c>
-      <c r="M45" s="171"/>
-      <c r="N45" s="174"/>
-      <c r="O45" s="175"/>
-    </row>
-    <row r="46" spans="2:16" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J45" s="77"/>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="10"/>
       <c r="C46" s="61">
         <v>0.75</v>
@@ -4570,15 +4460,9 @@
       <c r="H46" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J46" s="120"/>
-      <c r="L46" s="170" t="s">
-        <v>185</v>
-      </c>
-      <c r="M46" s="171"/>
-      <c r="N46" s="174"/>
-      <c r="O46" s="175"/>
-    </row>
-    <row r="47" spans="2:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="J46" s="77"/>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="10"/>
       <c r="C47" s="61">
         <v>0.85</v>
@@ -4595,13 +4479,9 @@
       <c r="H47" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J47" s="120"/>
-      <c r="L47" s="178"/>
-      <c r="M47" s="171"/>
-      <c r="N47" s="174"/>
-      <c r="O47" s="175"/>
-    </row>
-    <row r="48" spans="2:16" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J47" s="77"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
       <c r="C48" s="61">
         <v>0.95</v>
@@ -4618,15 +4498,9 @@
       <c r="H48" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J48" s="120"/>
-      <c r="L48" s="170" t="s">
-        <v>184</v>
-      </c>
-      <c r="M48" s="171"/>
-      <c r="N48" s="174"/>
-      <c r="O48" s="175"/>
-    </row>
-    <row r="49" spans="2:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="J48" s="77"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="10"/>
       <c r="C49" s="61" t="s">
         <v>180</v>
@@ -4641,13 +4515,9 @@
       <c r="H49" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J49" s="120"/>
-      <c r="L49" s="178"/>
-      <c r="M49" s="171"/>
-      <c r="N49" s="174"/>
-      <c r="O49" s="175"/>
-    </row>
-    <row r="50" spans="2:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J49" s="77"/>
+    </row>
+    <row r="50" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="10"/>
       <c r="C50" s="61" t="s">
         <v>180</v>
@@ -4662,62 +4532,58 @@
       <c r="H50" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J50" s="121"/>
-      <c r="L50" s="170"/>
-      <c r="M50" s="171"/>
-      <c r="N50" s="176"/>
-      <c r="O50" s="177"/>
-    </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="J50" s="78"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="10"/>
       <c r="C51" s="61" t="s">
         <v>180</v>
       </c>
       <c r="D51" s="63"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="10"/>
       <c r="C52" s="61" t="s">
         <v>180</v>
       </c>
       <c r="D52" s="63"/>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="10"/>
       <c r="C53" s="61" t="s">
         <v>180</v>
       </c>
       <c r="D53" s="63"/>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="10"/>
       <c r="C54" s="61" t="s">
         <v>180</v>
       </c>
       <c r="D54" s="63"/>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="10"/>
       <c r="C55" s="61" t="s">
         <v>180</v>
       </c>
       <c r="D55" s="63"/>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="10"/>
       <c r="C56" s="61" t="s">
         <v>180</v>
       </c>
       <c r="D56" s="63"/>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="10"/>
       <c r="C57" s="61" t="s">
         <v>180</v>
       </c>
       <c r="D57" s="63"/>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" s="12"/>
       <c r="C58" s="64" t="s">
         <v>180</v>
@@ -4725,14 +4591,27 @@
       <c r="D58" s="65"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="J33:J40"/>
-    <mergeCell ref="J42:J50"/>
-    <mergeCell ref="N34:N40"/>
-    <mergeCell ref="M34:M40"/>
-    <mergeCell ref="L34:L40"/>
-    <mergeCell ref="N43:O50"/>
-    <mergeCell ref="N42:O42"/>
+  <mergeCells count="41">
+    <mergeCell ref="J2:J22"/>
+    <mergeCell ref="P17:P20"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="N17:N20"/>
+    <mergeCell ref="L17:L20"/>
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="B2:D22"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="O34:O40"/>
     <mergeCell ref="P34:P40"/>
     <mergeCell ref="J24:J31"/>
@@ -4749,32 +4628,12 @@
     <mergeCell ref="O27:P27"/>
     <mergeCell ref="O28:P28"/>
     <mergeCell ref="O29:P29"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="B2:D22"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="J2:J22"/>
-    <mergeCell ref="P17:P20"/>
-    <mergeCell ref="O17:O20"/>
-    <mergeCell ref="N17:N20"/>
-    <mergeCell ref="L17:L20"/>
-    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="J33:J40"/>
+    <mergeCell ref="J42:J50"/>
+    <mergeCell ref="N34:N40"/>
+    <mergeCell ref="M34:M40"/>
+    <mergeCell ref="L34:L40"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L49" xr:uid="{08959939-6A52-44E8-85B5-FE86F357123D}">
-      <formula1>$R$3:$R$31</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="5">
@@ -4786,7 +4645,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{743D23BA-875A-41E5-B597-5B2C8A5A8364}">
           <x14:formula1>
             <xm:f>Treinamento!$A$2:$A$5</xm:f>
@@ -4811,12 +4670,6 @@
           </x14:formula1>
           <xm:sqref>P16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{AD05FC42-F88E-439F-A63A-78FD21B5EA53}">
-          <x14:formula1>
-            <xm:f>Outros!$E$1:$E$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>L47</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -4825,30 +4678,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F9C691-1EF9-4764-A080-BE553620E14D}">
-  <sheetPr codeName="Planilha2"/>
   <dimension ref="B1:P31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" customWidth="1"/>
-    <col min="2" max="2" width="3.6640625" customWidth="1"/>
-    <col min="3" max="3" width="1.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="10.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.6640625" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="1.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="0.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="76" t="s">
+    <row r="1" spans="2:16" ht="0.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="133" t="s">
         <v>89</v>
       </c>
       <c r="D2" s="26" t="s">
@@ -4879,8 +4731,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="77"/>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="134"/>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
@@ -4891,8 +4743,8 @@
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="77"/>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="134"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
       <c r="F4" s="26"/>
@@ -4903,60 +4755,60 @@
       <c r="K4" s="26"/>
       <c r="L4" s="26"/>
     </row>
-    <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="77"/>
-    </row>
-    <row r="6" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="77"/>
-      <c r="D6" s="160" t="s">
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="134"/>
+    </row>
+    <row r="6" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="134"/>
+      <c r="D6" s="142" t="s">
         <v>131</v>
       </c>
-      <c r="E6" s="161"/>
-      <c r="F6" s="161"/>
-      <c r="G6" s="161"/>
-      <c r="H6" s="161"/>
-      <c r="I6" s="161"/>
-      <c r="J6" s="161"/>
-      <c r="K6" s="161"/>
-      <c r="L6" s="162"/>
-    </row>
-    <row r="7" spans="2:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="77"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="164"/>
-      <c r="F7" s="164"/>
-      <c r="G7" s="164"/>
-      <c r="H7" s="164"/>
-      <c r="I7" s="164"/>
-      <c r="J7" s="164"/>
-      <c r="K7" s="164"/>
-      <c r="L7" s="165"/>
-    </row>
-    <row r="8" spans="2:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="77"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="164"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="164"/>
-      <c r="H8" s="164"/>
-      <c r="I8" s="164"/>
-      <c r="J8" s="164"/>
-      <c r="K8" s="164"/>
-      <c r="L8" s="165"/>
-    </row>
-    <row r="9" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="77"/>
-    </row>
-    <row r="10" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="77"/>
-      <c r="D10" s="160" t="s">
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="143"/>
+      <c r="I6" s="143"/>
+      <c r="J6" s="143"/>
+      <c r="K6" s="143"/>
+      <c r="L6" s="144"/>
+    </row>
+    <row r="7" spans="2:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="134"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="146"/>
+      <c r="H7" s="146"/>
+      <c r="I7" s="146"/>
+      <c r="J7" s="146"/>
+      <c r="K7" s="146"/>
+      <c r="L7" s="147"/>
+    </row>
+    <row r="8" spans="2:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="134"/>
+      <c r="D8" s="145"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="146"/>
+      <c r="G8" s="146"/>
+      <c r="H8" s="146"/>
+      <c r="I8" s="146"/>
+      <c r="J8" s="146"/>
+      <c r="K8" s="146"/>
+      <c r="L8" s="147"/>
+    </row>
+    <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="134"/>
+    </row>
+    <row r="10" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="134"/>
+      <c r="D10" s="142" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="162"/>
-      <c r="F10" s="160" t="s">
+      <c r="E10" s="144"/>
+      <c r="F10" s="142" t="s">
         <v>97</v>
       </c>
-      <c r="G10" s="162"/>
+      <c r="G10" s="144"/>
       <c r="I10" s="43" t="s">
         <v>98</v>
       </c>
@@ -4970,18 +4822,18 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="77"/>
-      <c r="D11" s="166">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="134"/>
+      <c r="D11" s="148">
         <f>7+IF(Básico!P3&gt;0,Básico!P3*2,Básico!P3)</f>
         <v>7</v>
       </c>
-      <c r="E11" s="167"/>
-      <c r="F11" s="166">
+      <c r="E11" s="149"/>
+      <c r="F11" s="148">
         <f>D11-SUM(Armamento[Espaço])-SUM(Defesa[Espaço])-SUM(Acessórios[Espaço])</f>
         <v>7</v>
       </c>
-      <c r="G11" s="167"/>
+      <c r="G11" s="149"/>
       <c r="I11" s="46"/>
       <c r="J11" s="47" t="s">
         <v>144</v>
@@ -4993,12 +4845,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="78"/>
-      <c r="D12" s="168"/>
-      <c r="E12" s="169"/>
-      <c r="F12" s="168"/>
-      <c r="G12" s="169"/>
+    <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="135"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="150"/>
+      <c r="G12" s="151"/>
       <c r="I12" s="49"/>
       <c r="J12" s="50" t="s">
         <v>144</v>
@@ -5010,9 +4862,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="2:16" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="119" t="s">
+    <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="76" t="s">
         <v>100</v>
       </c>
       <c r="D14" s="52" t="s">
@@ -5027,108 +4879,108 @@
       <c r="G14" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="I14" s="151" t="s">
+      <c r="I14" s="152" t="s">
         <v>143</v>
       </c>
-      <c r="J14" s="152"/>
-      <c r="K14" s="152"/>
-      <c r="L14" s="153"/>
+      <c r="J14" s="153"/>
+      <c r="K14" s="153"/>
+      <c r="L14" s="154"/>
       <c r="N14" s="55"/>
       <c r="O14" s="55"/>
       <c r="P14" s="55"/>
     </row>
-    <row r="15" spans="2:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="120"/>
-      <c r="D15" s="157" t="str">
+    <row r="15" spans="2:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="77"/>
+      <c r="D15" s="160" t="str">
         <f>IFERROR(VLOOKUP(Básico!G10,Rank[],3,TRUE),"")</f>
         <v/>
       </c>
-      <c r="E15" s="157" t="str">
+      <c r="E15" s="160" t="str">
         <f>IF(D15&lt;&gt;"",SUM(Armamento[Custo])+SUM(Acessórios[Custo])+SUM(Defesa[Custo])+SUM(K16:L31),"")</f>
         <v/>
       </c>
-      <c r="F15" s="157"/>
-      <c r="G15" s="157" t="str">
+      <c r="F15" s="160"/>
+      <c r="G15" s="160" t="str">
         <f>IF(D15&lt;&gt;"",D15-E15-F15,"")</f>
         <v/>
       </c>
-      <c r="I15" s="154" t="s">
+      <c r="I15" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="J15" s="155"/>
-      <c r="K15" s="155" t="s">
+      <c r="J15" s="156"/>
+      <c r="K15" s="156" t="s">
         <v>142</v>
       </c>
-      <c r="L15" s="156"/>
+      <c r="L15" s="157"/>
       <c r="N15" s="55"/>
       <c r="O15" s="55"/>
       <c r="P15" s="55"/>
     </row>
-    <row r="16" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="120"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="I16" s="148"/>
-      <c r="J16" s="149"/>
-      <c r="K16" s="149"/>
-      <c r="L16" s="150"/>
+    <row r="16" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="77"/>
+      <c r="D16" s="161"/>
+      <c r="E16" s="161"/>
+      <c r="F16" s="161"/>
+      <c r="G16" s="161"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="163"/>
       <c r="N16" s="55"/>
       <c r="O16" s="55"/>
       <c r="P16" s="55"/>
     </row>
-    <row r="17" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="120"/>
-      <c r="D17" s="158"/>
-      <c r="E17" s="158"/>
-      <c r="F17" s="158"/>
-      <c r="G17" s="158"/>
-      <c r="I17" s="148"/>
-      <c r="J17" s="149"/>
-      <c r="K17" s="149"/>
-      <c r="L17" s="150"/>
+    <row r="17" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="77"/>
+      <c r="D17" s="161"/>
+      <c r="E17" s="161"/>
+      <c r="F17" s="161"/>
+      <c r="G17" s="161"/>
+      <c r="I17" s="158"/>
+      <c r="J17" s="159"/>
+      <c r="K17" s="159"/>
+      <c r="L17" s="163"/>
       <c r="N17" s="55"/>
       <c r="O17" s="55"/>
       <c r="P17" s="55"/>
     </row>
-    <row r="18" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="120"/>
-      <c r="D18" s="158"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="158"/>
-      <c r="G18" s="158"/>
+    <row r="18" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="77"/>
+      <c r="D18" s="161"/>
+      <c r="E18" s="161"/>
+      <c r="F18" s="161"/>
+      <c r="G18" s="161"/>
       <c r="H18" s="57"/>
-      <c r="I18" s="148"/>
-      <c r="J18" s="149"/>
-      <c r="K18" s="149"/>
-      <c r="L18" s="150"/>
+      <c r="I18" s="158"/>
+      <c r="J18" s="159"/>
+      <c r="K18" s="159"/>
+      <c r="L18" s="163"/>
       <c r="N18" s="55"/>
       <c r="O18" s="55"/>
       <c r="P18" s="55"/>
     </row>
-    <row r="19" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="121"/>
-      <c r="D19" s="159"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159"/>
-      <c r="G19" s="159"/>
-      <c r="I19" s="148"/>
-      <c r="J19" s="149"/>
-      <c r="K19" s="149"/>
-      <c r="L19" s="150"/>
+    <row r="19" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="78"/>
+      <c r="D19" s="162"/>
+      <c r="E19" s="162"/>
+      <c r="F19" s="162"/>
+      <c r="G19" s="162"/>
+      <c r="I19" s="158"/>
+      <c r="J19" s="159"/>
+      <c r="K19" s="159"/>
+      <c r="L19" s="163"/>
       <c r="N19" s="55"/>
       <c r="O19" s="55"/>
       <c r="P19" s="55"/>
     </row>
-    <row r="20" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I20" s="148"/>
-      <c r="J20" s="149"/>
-      <c r="K20" s="149"/>
-      <c r="L20" s="150"/>
-    </row>
-    <row r="21" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="119" t="s">
+    <row r="20" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="158"/>
+      <c r="J20" s="159"/>
+      <c r="K20" s="159"/>
+      <c r="L20" s="163"/>
+    </row>
+    <row r="21" spans="2:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="76" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="40" t="s">
@@ -5140,121 +4992,138 @@
       <c r="F21" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="I21" s="148"/>
-      <c r="J21" s="149"/>
-      <c r="K21" s="149"/>
-      <c r="L21" s="150"/>
-    </row>
-    <row r="22" spans="2:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="120"/>
+      <c r="I21" s="158"/>
+      <c r="J21" s="159"/>
+      <c r="K21" s="159"/>
+      <c r="L21" s="163"/>
+    </row>
+    <row r="22" spans="2:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="77"/>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
       <c r="F22" s="26"/>
-      <c r="I22" s="148"/>
-      <c r="J22" s="149"/>
-      <c r="K22" s="149"/>
-      <c r="L22" s="150"/>
-    </row>
-    <row r="23" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="120"/>
+      <c r="I22" s="158"/>
+      <c r="J22" s="159"/>
+      <c r="K22" s="159"/>
+      <c r="L22" s="163"/>
+    </row>
+    <row r="23" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="77"/>
       <c r="D23" s="26"/>
       <c r="E23" s="56"/>
       <c r="F23" s="26"/>
-      <c r="I23" s="148"/>
-      <c r="J23" s="149"/>
-      <c r="K23" s="149"/>
-      <c r="L23" s="150"/>
-    </row>
-    <row r="24" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="120"/>
+      <c r="I23" s="158"/>
+      <c r="J23" s="159"/>
+      <c r="K23" s="159"/>
+      <c r="L23" s="163"/>
+    </row>
+    <row r="24" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="77"/>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
       <c r="F24" s="26"/>
-      <c r="I24" s="148"/>
-      <c r="J24" s="149"/>
-      <c r="K24" s="149"/>
-      <c r="L24" s="150"/>
-    </row>
-    <row r="25" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="120"/>
+      <c r="I24" s="158"/>
+      <c r="J24" s="159"/>
+      <c r="K24" s="159"/>
+      <c r="L24" s="163"/>
+    </row>
+    <row r="25" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="77"/>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
       <c r="F25" s="26"/>
-      <c r="I25" s="148"/>
-      <c r="J25" s="149"/>
-      <c r="K25" s="149"/>
-      <c r="L25" s="150"/>
-    </row>
-    <row r="26" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="120"/>
+      <c r="I25" s="158"/>
+      <c r="J25" s="159"/>
+      <c r="K25" s="159"/>
+      <c r="L25" s="163"/>
+    </row>
+    <row r="26" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="77"/>
       <c r="D26" s="26"/>
       <c r="E26" s="26"/>
       <c r="F26" s="26"/>
-      <c r="I26" s="148"/>
-      <c r="J26" s="149"/>
-      <c r="K26" s="149"/>
-      <c r="L26" s="150"/>
-    </row>
-    <row r="27" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="120"/>
+      <c r="I26" s="158"/>
+      <c r="J26" s="159"/>
+      <c r="K26" s="159"/>
+      <c r="L26" s="163"/>
+    </row>
+    <row r="27" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="77"/>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
       <c r="F27" s="26"/>
-      <c r="I27" s="148"/>
-      <c r="J27" s="149"/>
-      <c r="K27" s="149"/>
-      <c r="L27" s="150"/>
-    </row>
-    <row r="28" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="120"/>
+      <c r="I27" s="158"/>
+      <c r="J27" s="159"/>
+      <c r="K27" s="159"/>
+      <c r="L27" s="163"/>
+    </row>
+    <row r="28" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="77"/>
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
       <c r="F28" s="26"/>
-      <c r="I28" s="148"/>
-      <c r="J28" s="149"/>
-      <c r="K28" s="149"/>
-      <c r="L28" s="150"/>
-    </row>
-    <row r="29" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="120"/>
+      <c r="I28" s="158"/>
+      <c r="J28" s="159"/>
+      <c r="K28" s="159"/>
+      <c r="L28" s="163"/>
+    </row>
+    <row r="29" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="77"/>
       <c r="D29" s="26"/>
       <c r="E29" s="26"/>
       <c r="F29" s="26"/>
-      <c r="I29" s="148"/>
-      <c r="J29" s="149"/>
-      <c r="K29" s="149"/>
-      <c r="L29" s="150"/>
-    </row>
-    <row r="30" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="120"/>
+      <c r="I29" s="158"/>
+      <c r="J29" s="159"/>
+      <c r="K29" s="159"/>
+      <c r="L29" s="163"/>
+    </row>
+    <row r="30" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="77"/>
       <c r="D30" s="26"/>
       <c r="E30" s="26"/>
       <c r="F30" s="26"/>
-      <c r="I30" s="148"/>
-      <c r="J30" s="149"/>
-      <c r="K30" s="149"/>
-      <c r="L30" s="150"/>
-    </row>
-    <row r="31" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="121"/>
+      <c r="I30" s="158"/>
+      <c r="J30" s="159"/>
+      <c r="K30" s="159"/>
+      <c r="L30" s="163"/>
+    </row>
+    <row r="31" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="78"/>
       <c r="D31" s="26"/>
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
-      <c r="I31" s="145"/>
-      <c r="J31" s="146"/>
-      <c r="K31" s="146"/>
-      <c r="L31" s="147"/>
+      <c r="I31" s="164"/>
+      <c r="J31" s="165"/>
+      <c r="K31" s="165"/>
+      <c r="L31" s="166"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="D6:L6"/>
-    <mergeCell ref="D7:L7"/>
-    <mergeCell ref="D8:L8"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
     <mergeCell ref="B21:B31"/>
     <mergeCell ref="I14:L14"/>
     <mergeCell ref="I15:J15"/>
@@ -5271,31 +5140,14 @@
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="D6:L6"/>
+    <mergeCell ref="D7:L7"/>
+    <mergeCell ref="D8:L8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="F11:G12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="3">
@@ -5308,40 +5160,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F0E6FE-FAF1-4596-BE6E-48F9FAEB8363}">
-  <sheetPr codeName="Planilha3"/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>160</v>
       </c>
       <c r="B1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>161</v>
       </c>
       <c r="B2" t="s">
         <v>176</v>
-      </c>
-      <c r="E2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E3" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -5351,21 +5191,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87674E58-DEAC-40E7-862B-B789E20723ED}">
-  <sheetPr codeName="Planilha4"/>
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>132</v>
       </c>
@@ -5376,7 +5215,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>138</v>
       </c>
@@ -5387,7 +5226,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>137</v>
       </c>
@@ -5398,7 +5237,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>136</v>
       </c>
@@ -5409,7 +5248,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>135</v>
       </c>
@@ -5420,7 +5259,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>134</v>
       </c>
@@ -5431,7 +5270,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>139</v>
       </c>
@@ -5442,7 +5281,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>140</v>
       </c>
@@ -5463,7 +5302,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96AC2B5F-CCAA-4F35-ABBE-C6E25CFCBB47}">
-  <sheetPr codeName="Planilha5">
+  <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:B15"/>
@@ -5472,12 +5311,12 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>94</v>
       </c>
@@ -5485,7 +5324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>104</v>
       </c>
@@ -5493,7 +5332,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>106</v>
       </c>
@@ -5501,7 +5340,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>108</v>
       </c>
@@ -5509,7 +5348,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>110</v>
       </c>
@@ -5517,7 +5356,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>112</v>
       </c>
@@ -5525,7 +5364,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>114</v>
       </c>
@@ -5533,7 +5372,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>116</v>
       </c>
@@ -5541,7 +5380,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>118</v>
       </c>
@@ -5549,7 +5388,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>108</v>
       </c>
@@ -5557,7 +5396,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>121</v>
       </c>
@@ -5565,7 +5404,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>123</v>
       </c>
@@ -5573,7 +5412,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>125</v>
       </c>
@@ -5581,7 +5420,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>127</v>
       </c>
@@ -5589,7 +5428,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>129</v>
       </c>
@@ -5607,44 +5446,43 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427FCFF7-1B4F-4AB7-95D7-9067EE83BDCC}">
-  <sheetPr codeName="Planilha6"/>
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="39"/>
     </row>
   </sheetData>
@@ -5657,22 +5495,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A82ED28-5B50-4C09-9044-29010E67E478}">
-  <sheetPr codeName="Planilha7"/>
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>26</v>
       </c>
@@ -5695,7 +5532,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -5718,7 +5555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -5741,7 +5578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -5764,7 +5601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -5787,7 +5624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>

</xml_diff>